<commit_message>
Minor formatting fixes so these are visible in Excel
</commit_message>
<xml_diff>
--- a/examples/1_1_Metabolomics_Draft/Progenesis example.xlsx
+++ b/examples/1_1_Metabolomics_Draft/Progenesis example.xlsx
@@ -1,12 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\PSI\mzTab\Git\examples\1_1_Metabolomics_Draft\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet2" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -235,8 +243,7 @@
     <t>C18H28O4</t>
   </si>
   <si>
-    <t>O(C1=CC(=O)C(=C(C1=O)CCCCCCCCCCC)O)C | O([C@H]([C@@H](O)CC(=O)CC)CCCC[C@@H](O)c1ccccc1)C        
-</t>
+    <t>O(C1=CC(=O)C(=C(C1=O)CCCCCCCCCCC)O)C | O([C@H]([C@@H](O)CC(=O)CC)CCCC[C@@H](O)c1ccccc1)C</t>
   </si>
   <si>
     <t>InChI=1S/C18H28O4/</t>
@@ -395,31 +402,41 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -427,7 +444,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -460,84 +477,322 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U47"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="52.29"/>
-    <col customWidth="1" min="3" max="3" width="76.29"/>
+    <col min="2" max="2" width="52.28515625" customWidth="1"/>
+    <col min="3" max="3" width="76.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +819,7 @@
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -593,7 +848,7 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -622,7 +877,7 @@
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -651,7 +906,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -680,7 +935,7 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -709,7 +964,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
@@ -738,7 +993,7 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -767,7 +1022,7 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -796,7 +1051,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -825,7 +1080,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -854,7 +1109,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -883,7 +1138,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>2</v>
       </c>
@@ -912,7 +1167,7 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -939,7 +1194,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -968,7 +1223,7 @@
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
@@ -997,7 +1252,7 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1026,7 +1281,7 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1310,7 @@
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -1063,7 +1318,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="4">
-        <v>42556.0</v>
+        <v>42556</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1084,7 +1339,7 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>2</v>
       </c>
@@ -1113,7 +1368,7 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>2</v>
       </c>
@@ -1142,7 +1397,7 @@
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
@@ -1150,7 +1405,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="4">
-        <v>42556.0</v>
+        <v>42556</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1171,7 +1426,7 @@
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>2</v>
       </c>
@@ -1200,7 +1455,7 @@
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>2</v>
       </c>
@@ -1229,7 +1484,7 @@
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1250,7 +1505,7 @@
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>45</v>
       </c>
@@ -1311,12 +1566,12 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="8">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>64</v>
@@ -1325,7 +1580,7 @@
         <v>65</v>
       </c>
       <c r="E27" s="8">
-        <v>310.0816</v>
+        <v>310.08159999999998</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>66</v>
@@ -1343,7 +1598,7 @@
         <v>39.9</v>
       </c>
       <c r="K27" s="8">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="L27" s="9" t="s">
         <v>69</v>
@@ -1358,13 +1613,13 @@
         <v>1395.05</v>
       </c>
       <c r="P27" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="8">
         <v>1395.05</v>
       </c>
       <c r="R27" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S27" s="8" t="s">
         <v>70</v>
@@ -1372,12 +1627,12 @@
       <c r="T27" s="7"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" ht="18.75" customHeight="1">
+    <row r="28" spans="1:21" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="8">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>71</v>
@@ -1386,7 +1641,7 @@
         <v>72</v>
       </c>
       <c r="E28" s="8">
-        <v>308.19876</v>
+        <v>308.19875999999999</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>73</v>
@@ -1401,44 +1656,44 @@
         <v>39</v>
       </c>
       <c r="J28" s="8">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="K28" s="8">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="L28" s="9" t="s">
         <v>76</v>
       </c>
       <c r="M28" s="8">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="N28" s="8">
-        <v>800.0</v>
+        <v>800</v>
       </c>
       <c r="O28" s="8">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="P28" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q28" s="8">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="R28" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S28" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>63</v>
       </c>
       <c r="B29" s="8">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>77</v>
@@ -1447,7 +1702,7 @@
         <v>78</v>
       </c>
       <c r="E29" s="10">
-        <v>308.1065</v>
+        <v>308.10649999999998</v>
       </c>
       <c r="F29" s="8" t="s">
         <v>79</v>
@@ -1465,28 +1720,28 @@
         <v>17.2</v>
       </c>
       <c r="K29" s="8">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="L29" s="8" t="s">
         <v>78</v>
       </c>
       <c r="M29" s="8">
-        <v>900.0</v>
+        <v>900</v>
       </c>
       <c r="N29" s="8">
-        <v>850.0</v>
+        <v>850</v>
       </c>
       <c r="O29" s="8">
-        <v>900.0</v>
+        <v>900</v>
       </c>
       <c r="P29" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="Q29" s="8">
-        <v>850.0</v>
+        <v>850</v>
       </c>
       <c r="R29" s="8">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S29" s="8" t="s">
         <v>82</v>
@@ -1494,7 +1749,7 @@
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>83</v>
       </c>
@@ -1541,18 +1796,18 @@
       <c r="T31" s="12"/>
       <c r="U31" s="12"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B32" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D32" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>94</v>
@@ -1570,7 +1825,7 @@
         <v>6.29</v>
       </c>
       <c r="J32" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K32" s="13">
         <v>805.16</v>
@@ -1588,24 +1843,24 @@
       <c r="T32" s="12"/>
       <c r="U32" s="12"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B33" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D33" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>95</v>
       </c>
       <c r="F33" s="13">
-        <v>349.179201</v>
+        <v>349.17920099999998</v>
       </c>
       <c r="G33" s="13">
         <v>6.23</v>
@@ -1617,7 +1872,7 @@
         <v>6.27</v>
       </c>
       <c r="J33" s="13">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K33" s="13">
         <v>446.9</v>
@@ -1635,24 +1890,24 @@
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B34" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D34" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>96</v>
       </c>
       <c r="F34" s="13">
-        <v>333.07067</v>
+        <v>333.07067000000001</v>
       </c>
       <c r="G34" s="13">
         <v>6.22</v>
@@ -1664,13 +1919,13 @@
         <v>6.24</v>
       </c>
       <c r="J34" s="13">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K34" s="13">
-        <v>143.0</v>
+        <v>143</v>
       </c>
       <c r="L34" s="13">
-        <v>143.0</v>
+        <v>143</v>
       </c>
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
@@ -1682,24 +1937,24 @@
       <c r="T34" s="12"/>
       <c r="U34" s="12"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B35" s="13">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D35" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>78</v>
       </c>
       <c r="F35" s="13">
-        <v>309.2063673</v>
+        <v>309.20636730000001</v>
       </c>
       <c r="G35" s="13">
         <v>7.12</v>
@@ -1714,10 +1969,10 @@
         <v>97</v>
       </c>
       <c r="K35" s="13">
-        <v>1000.0</v>
+        <v>1000</v>
       </c>
       <c r="L35" s="13">
-        <v>800.0</v>
+        <v>800</v>
       </c>
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
@@ -1729,24 +1984,24 @@
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B36" s="13">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D36" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>95</v>
       </c>
       <c r="F36" s="13">
-        <v>347.069863068203</v>
+        <v>347.06986306820301</v>
       </c>
       <c r="G36" s="13">
         <v>7.11</v>
@@ -1758,13 +2013,13 @@
         <v>7.17</v>
       </c>
       <c r="J36" s="13">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="K36" s="13">
-        <v>400.0</v>
+        <v>400</v>
       </c>
       <c r="L36" s="13">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="M36" s="12"/>
       <c r="N36" s="12"/>
@@ -1776,24 +2031,24 @@
       <c r="T36" s="12"/>
       <c r="U36" s="12"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B37" s="13">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D37" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>94</v>
       </c>
       <c r="F37" s="13">
-        <v>309.11474</v>
+        <v>309.11473999999998</v>
       </c>
       <c r="G37" s="13">
         <v>7.12</v>
@@ -1805,13 +2060,13 @@
         <v>7.22</v>
       </c>
       <c r="J37" s="13">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="K37" s="13">
-        <v>600.0</v>
+        <v>600</v>
       </c>
       <c r="L37" s="13">
-        <v>680.0</v>
+        <v>680</v>
       </c>
       <c r="M37" s="12"/>
       <c r="N37" s="12"/>
@@ -1823,27 +2078,27 @@
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
         <v>93</v>
       </c>
       <c r="B38" s="13">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>78</v>
       </c>
       <c r="D38" s="13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>78</v>
       </c>
       <c r="F38" s="13">
-        <v>323.281963751238</v>
+        <v>323.28196375123798</v>
       </c>
       <c r="G38" s="13">
-        <v>8.2</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="H38" s="13">
         <v>8.16</v>
@@ -1855,10 +2110,10 @@
         <v>78</v>
       </c>
       <c r="K38" s="13">
-        <v>320.0</v>
+        <v>320</v>
       </c>
       <c r="L38" s="13">
-        <v>130.0</v>
+        <v>130</v>
       </c>
       <c r="M38" s="12"/>
       <c r="N38" s="12"/>
@@ -1870,11 +2125,11 @@
       <c r="T38" s="12"/>
       <c r="U38" s="12"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>98</v>
       </c>
@@ -1939,12 +2194,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B41" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>64</v>
@@ -1968,13 +2223,13 @@
         <v>311.08954</v>
       </c>
       <c r="J41" s="15">
-        <v>310.0816</v>
+        <v>310.08159999999998</v>
       </c>
       <c r="K41" s="15">
         <v>6.22</v>
       </c>
       <c r="L41" s="15">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M41" s="16" t="s">
         <v>69</v>
@@ -1989,7 +2244,7 @@
         <v>39.9</v>
       </c>
       <c r="Q41" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R41" s="15" t="s">
         <v>78</v>
@@ -1998,18 +2253,18 @@
         <v>94</v>
       </c>
       <c r="T41" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="U41" s="15">
         <v>6.25</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B42" s="15">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>64</v>
@@ -2027,19 +2282,19 @@
         <v>65</v>
       </c>
       <c r="H42" s="15">
-        <v>349.179201</v>
+        <v>349.17920099999998</v>
       </c>
       <c r="I42" s="15">
-        <v>349.179201</v>
+        <v>349.17920099999998</v>
       </c>
       <c r="J42" s="15">
-        <v>310.0816</v>
+        <v>310.08159999999998</v>
       </c>
       <c r="K42" s="15">
         <v>6.23</v>
       </c>
       <c r="L42" s="15">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M42" s="16" t="s">
         <v>69</v>
@@ -2054,7 +2309,7 @@
         <v>39.9</v>
       </c>
       <c r="Q42" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R42" s="15" t="s">
         <v>78</v>
@@ -2063,18 +2318,18 @@
         <v>95</v>
       </c>
       <c r="T42" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="U42" s="15">
         <v>6.25</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B43" s="15">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>112</v>
@@ -2092,19 +2347,19 @@
         <v>65</v>
       </c>
       <c r="H43" s="15">
-        <v>333.07067</v>
+        <v>333.07067000000001</v>
       </c>
       <c r="I43" s="15">
-        <v>333.07067</v>
+        <v>333.07067000000001</v>
       </c>
       <c r="J43" s="15">
-        <v>310.0816</v>
+        <v>310.08159999999998</v>
       </c>
       <c r="K43" s="15">
         <v>6.22</v>
       </c>
       <c r="L43" s="15">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M43" s="16" t="s">
         <v>69</v>
@@ -2119,7 +2374,7 @@
         <v>39.96</v>
       </c>
       <c r="Q43" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R43" s="15" t="s">
         <v>78</v>
@@ -2128,18 +2383,18 @@
         <v>96</v>
       </c>
       <c r="T43" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="U43" s="15">
         <v>6.25</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B44" s="15">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="C44" s="15" t="s">
         <v>114</v>
@@ -2157,19 +2412,19 @@
         <v>117</v>
       </c>
       <c r="H44" s="15">
-        <v>309.2063673</v>
+        <v>309.20636730000001</v>
       </c>
       <c r="I44" s="15">
-        <v>309.206701</v>
+        <v>309.20670100000001</v>
       </c>
       <c r="J44" s="15">
-        <v>308.198761</v>
+        <v>308.19876099999999</v>
       </c>
       <c r="K44" s="15">
         <v>7.04</v>
       </c>
       <c r="L44" s="15">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M44" s="16" t="s">
         <v>76</v>
@@ -2184,7 +2439,7 @@
         <v>39.9</v>
       </c>
       <c r="Q44" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R44" s="15" t="s">
         <v>78</v>
@@ -2193,18 +2448,18 @@
         <v>94</v>
       </c>
       <c r="T44" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="U44" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B45" s="15">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="C45" s="15" t="s">
         <v>119</v>
@@ -2222,19 +2477,19 @@
         <v>122</v>
       </c>
       <c r="H45" s="15">
-        <v>309.2063673</v>
+        <v>309.20636730000001</v>
       </c>
       <c r="I45" s="15">
-        <v>309.206701</v>
+        <v>309.20670100000001</v>
       </c>
       <c r="J45" s="15">
-        <v>308.198761</v>
+        <v>308.19876099999999</v>
       </c>
       <c r="K45" s="15">
         <v>7.04</v>
       </c>
       <c r="L45" s="15">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M45" s="16" t="s">
         <v>76</v>
@@ -2249,7 +2504,7 @@
         <v>39.9</v>
       </c>
       <c r="Q45" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R45" s="15" t="s">
         <v>78</v>
@@ -2258,18 +2513,18 @@
         <v>94</v>
       </c>
       <c r="T45" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="U45" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B46" s="15">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>77</v>
@@ -2287,19 +2542,19 @@
         <v>78</v>
       </c>
       <c r="H46" s="15">
-        <v>347.069863068203</v>
+        <v>347.06986306820301</v>
       </c>
       <c r="I46" s="15">
         <v>309.11444</v>
       </c>
       <c r="J46" s="15">
-        <v>308.1065</v>
+        <v>308.10649999999998</v>
       </c>
       <c r="K46" s="15">
         <v>7.11</v>
       </c>
       <c r="L46" s="15">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M46" s="15" t="s">
         <v>78</v>
@@ -2314,7 +2569,7 @@
         <v>17.2</v>
       </c>
       <c r="Q46" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R46" s="15" t="s">
         <v>78</v>
@@ -2323,18 +2578,18 @@
         <v>95</v>
       </c>
       <c r="T46" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="U46" s="15" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:21" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B47" s="15">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>77</v>
@@ -2352,19 +2607,19 @@
         <v>78</v>
       </c>
       <c r="H47" s="15">
-        <v>309.11474</v>
+        <v>309.11473999999998</v>
       </c>
       <c r="I47" s="15">
-        <v>347.2048</v>
+        <v>347.20479999999998</v>
       </c>
       <c r="J47" s="15">
-        <v>308.1065</v>
+        <v>308.10649999999998</v>
       </c>
       <c r="K47" s="15">
         <v>7.12</v>
       </c>
       <c r="L47" s="15">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M47" s="15" t="s">
         <v>78</v>
@@ -2379,7 +2634,7 @@
         <v>17.2</v>
       </c>
       <c r="Q47" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="R47" s="15" t="s">
         <v>78</v>
@@ -2388,7 +2643,7 @@
         <v>94</v>
       </c>
       <c r="T47" s="15">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="U47" s="15" t="s">
         <v>78</v>
@@ -2396,14 +2651,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="L27"/>
-    <hyperlink r:id="rId2" ref="L28"/>
-    <hyperlink r:id="rId3" ref="M41"/>
-    <hyperlink r:id="rId4" ref="M42"/>
-    <hyperlink r:id="rId5" ref="M43"/>
-    <hyperlink r:id="rId6" ref="M44"/>
-    <hyperlink r:id="rId7" ref="M45"/>
+    <hyperlink ref="L27" r:id="rId1"/>
+    <hyperlink ref="L28" r:id="rId2"/>
+    <hyperlink ref="M41" r:id="rId3"/>
+    <hyperlink ref="M42" r:id="rId4"/>
+    <hyperlink ref="M43" r:id="rId5"/>
+    <hyperlink ref="M44" r:id="rId6"/>
+    <hyperlink ref="M45" r:id="rId7"/>
   </hyperlinks>
-  <drawing r:id="rId8"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>